<commit_message>
test from sandra, first commit
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>설명</t>
   </si>
@@ -89,6 +89,10 @@
   </si>
   <si>
     <t>dcbfcb3c876d87d92635ff4deebf110b</t>
+  </si>
+  <si>
+    <t>ddddd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -197,7 +201,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -239,7 +243,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,7 +278,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -483,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -609,6 +613,11 @@
       </c>
       <c r="B12" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>